<commit_message>
Added an explanation for each test query.
</commit_message>
<xml_diff>
--- a/Recommendations_Output.xlsx
+++ b/Recommendations_Output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,6 +449,11 @@
           <t>Similarity_Score</t>
         </is>
       </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Explanation</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -464,6 +469,11 @@
       <c r="C2" t="n">
         <v>0.335</v>
       </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Matched due to overlap in key terms: java, can, an, looking, assessment, that, minutes, with, in, who</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -479,6 +489,11 @@
       <c r="C3" t="n">
         <v>0.335</v>
       </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Matched due to overlap in key terms: java, can, an, looking, assessment, that, minutes, with, in, who</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -493,6 +508,11 @@
       </c>
       <c r="C4" t="n">
         <v>0.335</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Matched due to overlap in key terms: java, can, an, looking, assessment, that, minutes, with, in, who</t>
+        </is>
       </c>
     </row>
     <row r="5">
@@ -547,6 +567,11 @@
       <c r="C5" t="n">
         <v>0.89</v>
       </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Matched due to overlap in key terms: insight, looking, science, huge, flexibility, market, ago, candidates, key, best, develop, touch, lead, diversity, workplace, sure, find, excellent, through, business, with, lifeatshl, careeropportunities, than, no, success, years, family, coaching, job, one, is, ability, services, future, around, an, shlhiringtalent, s, solution, transform, talent, are, knowledgeable, description, how, to, become, contribute, experience, us, flexible, careersatshl, fabric, join, workplaces, as, development, encourage, world, inclusion, breaking, something, engineer, me, started, adjustments, possible, career, ongoing, you, your, out, at, about, takes, there, we, goals, inclusivity, employer, shl, when, industry, offer, the, businesses, growth, and, experiences, time, guidance, process, jobopportunities, knowledge, others, shaping, possibilities, from, opportunity, unlock, insights, fun, equity, accessibility, that, power, threads, choose, desirable, more, product, doing, care, technology, get, this, greatest, inspired, continue, products, path, new, people, so, help, by, make, equal, 40, where, culture, scale, be, community, work, offered, assessment, transformational, lives, will, intrinsic, off, making, in, collaboration, acquisition, outcomes, team, package, employee, achieve, application, do, all, better, friendly, benefits, ll, manager, launches, what, on, transformation, ground, a, investment, dei, for, applications, answers, can, part, support, inclusive, essential, inspire, of, range, recruitment, our, diverse, currently, powerhouse</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -600,6 +625,11 @@
       <c r="C6" t="n">
         <v>0.89</v>
       </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Matched due to overlap in key terms: insight, looking, science, huge, flexibility, market, ago, candidates, key, best, develop, touch, lead, diversity, workplace, sure, find, excellent, through, business, with, lifeatshl, careeropportunities, than, no, success, years, family, coaching, job, one, is, ability, services, future, around, an, shlhiringtalent, s, solution, transform, talent, are, knowledgeable, description, how, to, become, contribute, experience, us, flexible, careersatshl, fabric, join, workplaces, as, development, encourage, world, inclusion, breaking, something, engineer, me, started, adjustments, possible, career, ongoing, you, your, out, at, about, takes, there, we, goals, inclusivity, employer, shl, when, industry, offer, the, businesses, growth, and, experiences, time, guidance, process, jobopportunities, knowledge, others, shaping, possibilities, from, opportunity, unlock, insights, fun, equity, accessibility, that, power, threads, choose, desirable, more, product, doing, care, technology, get, this, greatest, inspired, continue, products, path, new, people, so, help, by, make, equal, 40, where, culture, scale, be, community, work, offered, assessment, transformational, lives, will, intrinsic, off, making, in, collaboration, acquisition, outcomes, team, package, employee, achieve, application, do, all, better, friendly, benefits, ll, manager, launches, what, on, transformation, ground, a, investment, dei, for, applications, answers, can, part, support, inclusive, essential, inspire, of, range, recruitment, our, diverse, currently, powerhouse</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -653,6 +683,11 @@
       <c r="C7" t="n">
         <v>0.89</v>
       </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Matched due to overlap in key terms: insight, looking, science, huge, flexibility, market, ago, candidates, key, best, develop, touch, lead, diversity, workplace, sure, find, excellent, through, business, with, lifeatshl, careeropportunities, than, no, success, years, family, coaching, job, one, is, ability, services, future, around, an, shlhiringtalent, s, solution, transform, talent, are, knowledgeable, description, how, to, become, contribute, experience, us, flexible, careersatshl, fabric, join, workplaces, as, development, encourage, world, inclusion, breaking, something, engineer, me, started, adjustments, possible, career, ongoing, you, your, out, at, about, takes, there, we, goals, inclusivity, employer, shl, when, industry, offer, the, businesses, growth, and, experiences, time, guidance, process, jobopportunities, knowledge, others, shaping, possibilities, from, opportunity, unlock, insights, fun, equity, accessibility, that, power, threads, choose, desirable, more, product, doing, care, technology, get, this, greatest, inspired, continue, products, path, new, people, so, help, by, make, equal, 40, where, culture, scale, be, community, work, offered, assessment, transformational, lives, will, intrinsic, off, making, in, collaboration, acquisition, outcomes, team, package, employee, achieve, application, do, all, better, friendly, benefits, ll, manager, launches, what, on, transformation, ground, a, investment, dei, for, applications, answers, can, part, support, inclusive, essential, inspire, of, range, recruitment, our, diverse, currently, powerhouse</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -668,6 +703,11 @@
       <c r="C8" t="n">
         <v>0.244</v>
       </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Matched due to overlap in key terms: what, applications, an, and, are, to, for, tests</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -683,6 +723,11 @@
       <c r="C9" t="n">
         <v>0.244</v>
       </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Matched due to overlap in key terms: what, applications, an, and, are, to, for, tests</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -697,6 +742,11 @@
       </c>
       <c r="C10" t="n">
         <v>0.244</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Matched due to overlap in key terms: what, applications, an, and, are, to, for, tests</t>
+        </is>
       </c>
     </row>
     <row r="11">
@@ -772,6 +822,11 @@
       <c r="C11" t="n">
         <v>0.771</v>
       </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Matched due to overlap in key terms: insight, science, want, huge, flexibility, market, ago, candidates, key, best, develop, touch, lead, diversity, design, workplace, sure, find, excellent, through, business, with, lifeatshl, than, no, success, years, family, coaching, job, or, one, is, ability, services, around, an, s, solution, transform, talent, are, knowledgeable, description, how, to, become, experience, us, flexible, careersatshl, fabric, join, workplaces, as, development, encourage, world, inclusion, breaking, something, started, getting, adjustments, possible, career, ongoing, you, your, out, at, ready, about, takes, there, we, goals, inclusivity, employer, shl, when, industry, offer, the, businesses, growth, and, required, experiences, time, guidance, process, knowledge, others, possibilities, test, from, opportunity, unlock, quality, insights, fun, equity, accessibility, that, solutions, power, threads, choose, desirable, more, product, care, technology, get, this, greatest, inspired, continue, products, path, new, people, so, help, by, make, equal, functional, 40, where, culture, scale, be, work, offered, transformational, lives, will, intrinsic, off, making, in, collaboration, acquisition, create, team, package, outcomes, employee, achieve, application, do, all, better, benefits, ll, manager, launches, what, on, transformation, ground, a, investment, dei, long, for, applications, answers, can, part, support, inclusive, inspire, creating, strong, of, range, recruitment, our, diverse, currently, powerhouse</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -846,6 +901,11 @@
       <c r="C12" t="n">
         <v>0.771</v>
       </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Matched due to overlap in key terms: insight, science, want, huge, flexibility, market, ago, candidates, key, best, develop, touch, lead, diversity, design, workplace, sure, find, excellent, through, business, with, lifeatshl, than, no, success, years, family, coaching, job, or, one, is, ability, services, around, an, s, solution, transform, talent, are, knowledgeable, description, how, to, become, experience, us, flexible, careersatshl, fabric, join, workplaces, as, development, encourage, world, inclusion, breaking, something, started, getting, adjustments, possible, career, ongoing, you, your, out, at, ready, about, takes, there, we, goals, inclusivity, employer, shl, when, industry, offer, the, businesses, growth, and, required, experiences, time, guidance, process, knowledge, others, possibilities, test, from, opportunity, unlock, quality, insights, fun, equity, accessibility, that, solutions, power, threads, choose, desirable, more, product, care, technology, get, this, greatest, inspired, continue, products, path, new, people, so, help, by, make, equal, functional, 40, where, culture, scale, be, work, offered, transformational, lives, will, intrinsic, off, making, in, collaboration, acquisition, create, team, package, outcomes, employee, achieve, application, do, all, better, benefits, ll, manager, launches, what, on, transformation, ground, a, investment, dei, long, for, applications, answers, can, part, support, inclusive, inspire, creating, strong, of, range, recruitment, our, diverse, currently, powerhouse</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -920,6 +980,11 @@
       <c r="C13" t="n">
         <v>0.771</v>
       </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Matched due to overlap in key terms: insight, science, want, huge, flexibility, market, ago, candidates, key, best, develop, touch, lead, diversity, design, workplace, sure, find, excellent, through, business, with, lifeatshl, than, no, success, years, family, coaching, job, or, one, is, ability, services, around, an, s, solution, transform, talent, are, knowledgeable, description, how, to, become, experience, us, flexible, careersatshl, fabric, join, workplaces, as, development, encourage, world, inclusion, breaking, something, started, getting, adjustments, possible, career, ongoing, you, your, out, at, ready, about, takes, there, we, goals, inclusivity, employer, shl, when, industry, offer, the, businesses, growth, and, required, experiences, time, guidance, process, knowledge, others, possibilities, test, from, opportunity, unlock, quality, insights, fun, equity, accessibility, that, solutions, power, threads, choose, desirable, more, product, care, technology, get, this, greatest, inspired, continue, products, path, new, people, so, help, by, make, equal, functional, 40, where, culture, scale, be, work, offered, transformational, lives, will, intrinsic, off, making, in, collaboration, acquisition, create, team, package, outcomes, employee, achieve, application, do, all, better, benefits, ll, manager, launches, what, on, transformation, ground, a, investment, dei, long, for, applications, answers, can, part, support, inclusive, inspire, creating, strong, of, range, recruitment, our, diverse, currently, powerhouse</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -935,6 +1000,11 @@
       <c r="C14" t="n">
         <v>0.335</v>
       </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Matched due to overlap in key terms: an, new, graduates, i, sales, in, for, my</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -950,6 +1020,11 @@
       <c r="C15" t="n">
         <v>0.335</v>
       </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Matched due to overlap in key terms: an, new, graduates, i, sales, in, for, my</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -964,6 +1039,11 @@
       </c>
       <c r="C16" t="n">
         <v>0.335</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Matched due to overlap in key terms: an, new, graduates, i, sales, in, for, my</t>
+        </is>
       </c>
     </row>
     <row r="17">
@@ -994,6 +1074,11 @@
       <c r="C17" t="n">
         <v>0.463</v>
       </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Matched due to overlap in key terms: other, culture, be, content, best, opportunity, in, e, team, working, driven, that, continuous, with, about, on, we, provide, organization, communication, product, a, members, individuals, one, is, the, for, com, leading, s, and, are, description, of, to, executing, equal, experience, position</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1023,6 +1108,11 @@
       <c r="C18" t="n">
         <v>0.463</v>
       </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Matched due to overlap in key terms: other, culture, be, content, best, opportunity, in, e, team, working, driven, that, continuous, with, about, on, we, provide, organization, communication, product, a, members, individuals, one, is, the, for, com, leading, s, and, are, description, of, to, executing, equal, experience, position</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1052,6 +1142,11 @@
       <c r="C19" t="n">
         <v>0.463</v>
       </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Matched due to overlap in key terms: other, culture, be, content, best, opportunity, in, e, team, working, driven, that, continuous, with, about, on, we, provide, organization, communication, product, a, members, individuals, one, is, the, for, com, leading, s, and, are, description, of, to, executing, equal, experience, position</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1067,6 +1162,11 @@
       <c r="C20" t="n">
         <v>0.495</v>
       </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Matched due to overlap in key terms: and, want, expertise, a, years, i, hire, of, to, with, experience, in</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1082,6 +1182,11 @@
       <c r="C21" t="n">
         <v>0.495</v>
       </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Matched due to overlap in key terms: and, want, expertise, a, years, i, hire, of, to, with, experience, in</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1096,6 +1201,11 @@
       </c>
       <c r="C22" t="n">
         <v>0.495</v>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Matched due to overlap in key terms: and, want, expertise, a, years, i, hire, of, to, with, experience, in</t>
+        </is>
       </c>
     </row>
     <row r="23">
@@ -1146,6 +1256,11 @@
       <c r="C23" t="n">
         <v>0.834</v>
       </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Matched due to overlap in key terms: insight, looking, science, huge, flexibility, market, ago, candidates, key, best, develop, touch, lead, diversity, workplace, sure, find, excellent, through, business, with, lifeatshl, management, than, no, success, years, family, coaching, job, or, one, is, ability, services, around, an, shlhiringtalent, s, transform, talent, are, knowledgeable, description, how, to, become, experience, below, us, flexible, careersatshl, fabric, join, workplaces, as, development, encourage, world, inclusion, breaking, something, me, started, adjustments, possible, career, ongoing, you, your, out, at, about, takes, there, we, providing, goals, inclusivity, employer, shl, when, industry, offer, the, businesses, growth, and, experiences, time, guidance, process, knowledge, others, possibilities, 1, from, opportunity, unlock, quality, insights, fun, equity, accessibility, that, power, processes, threads, choose, more, product, doing, care, technology, get, this, greatest, inspired, continue, products, path, new, people, so, help, by, make, equal, 40, where, culture, scale, be, work, offered, assessment, transformational, lives, will, intrinsic, off, making, in, collaboration, acquisition, outcomes, team, package, employee, achieve, application, do, all, better, friendly, benefits, ll, manager, launches, what, on, transformation, ground, a, investment, dei, for, applications, answers, can, part, support, inclusive, inspire, strong, of, range, recruitment, our, diverse, currently, powerhouse</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1195,6 +1310,11 @@
       <c r="C24" t="n">
         <v>0.834</v>
       </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Matched due to overlap in key terms: insight, looking, science, huge, flexibility, market, ago, candidates, key, best, develop, touch, lead, diversity, workplace, sure, find, excellent, through, business, with, lifeatshl, management, than, no, success, years, family, coaching, job, or, one, is, ability, services, around, an, shlhiringtalent, s, transform, talent, are, knowledgeable, description, how, to, become, experience, below, us, flexible, careersatshl, fabric, join, workplaces, as, development, encourage, world, inclusion, breaking, something, me, started, adjustments, possible, career, ongoing, you, your, out, at, about, takes, there, we, providing, goals, inclusivity, employer, shl, when, industry, offer, the, businesses, growth, and, experiences, time, guidance, process, knowledge, others, possibilities, 1, from, opportunity, unlock, quality, insights, fun, equity, accessibility, that, power, processes, threads, choose, more, product, doing, care, technology, get, this, greatest, inspired, continue, products, path, new, people, so, help, by, make, equal, 40, where, culture, scale, be, work, offered, assessment, transformational, lives, will, intrinsic, off, making, in, collaboration, acquisition, outcomes, team, package, employee, achieve, application, do, all, better, friendly, benefits, ll, manager, launches, what, on, transformation, ground, a, investment, dei, for, applications, answers, can, part, support, inclusive, inspire, strong, of, range, recruitment, our, diverse, currently, powerhouse</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1244,6 +1364,11 @@
       <c r="C25" t="n">
         <v>0.834</v>
       </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Matched due to overlap in key terms: insight, looking, science, huge, flexibility, market, ago, candidates, key, best, develop, touch, lead, diversity, workplace, sure, find, excellent, through, business, with, lifeatshl, management, than, no, success, years, family, coaching, job, or, one, is, ability, services, around, an, shlhiringtalent, s, transform, talent, are, knowledgeable, description, how, to, become, experience, below, us, flexible, careersatshl, fabric, join, workplaces, as, development, encourage, world, inclusion, breaking, something, me, started, adjustments, possible, career, ongoing, you, your, out, at, about, takes, there, we, providing, goals, inclusivity, employer, shl, when, industry, offer, the, businesses, growth, and, experiences, time, guidance, process, knowledge, others, possibilities, 1, from, opportunity, unlock, quality, insights, fun, equity, accessibility, that, power, processes, threads, choose, more, product, doing, care, technology, get, this, greatest, inspired, continue, products, path, new, people, so, help, by, make, equal, 40, where, culture, scale, be, work, offered, assessment, transformational, lives, will, intrinsic, off, making, in, collaboration, acquisition, outcomes, team, package, employee, achieve, application, do, all, better, friendly, benefits, ll, manager, launches, what, on, transformation, ground, a, investment, dei, for, applications, answers, can, part, support, inclusive, inspire, strong, of, range, recruitment, our, diverse, currently, powerhouse</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1290,6 +1415,11 @@
       <c r="C26" t="n">
         <v>0.59</v>
       </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Matched due to overlap in key terms: manage, us, other, flexible, be, work, skills, deliver, as, not, will, professional, in, team, responsibilities, working, i, that, building, with, benefits, at, management, about, on, issues, providing, we, provide, communication, product, years, more, based, employer, sales, a, technology, or, when, this, is, ability, role, the, for, relevant, services, businesses, an, expert, leading, s, and, organizational, support, internal, opportunities, are, ensuring, teams, 2, by, strong, of, to, equal, experience</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1336,6 +1466,11 @@
       <c r="C27" t="n">
         <v>0.59</v>
       </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Matched due to overlap in key terms: manage, us, other, flexible, be, work, skills, deliver, as, not, will, professional, in, team, responsibilities, working, i, that, building, with, benefits, at, management, about, on, issues, providing, we, provide, communication, product, years, more, based, employer, sales, a, technology, or, when, this, is, ability, role, the, for, relevant, services, businesses, an, expert, leading, s, and, organizational, support, internal, opportunities, are, ensuring, teams, 2, by, strong, of, to, equal, experience</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1382,6 +1517,11 @@
       <c r="C28" t="n">
         <v>0.59</v>
       </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Matched due to overlap in key terms: manage, us, other, flexible, be, work, skills, deliver, as, not, will, professional, in, team, responsibilities, working, i, that, building, with, benefits, at, management, about, on, issues, providing, we, provide, communication, product, years, more, based, employer, sales, a, technology, or, when, this, is, ability, role, the, for, relevant, services, businesses, an, expert, leading, s, and, organizational, support, internal, opportunities, are, ensuring, teams, 2, by, strong, of, to, equal, experience</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Added user friendly features.
</commit_message>
<xml_diff>
--- a/Recommendations_Output.xlsx
+++ b/Recommendations_Output.xlsx
@@ -7,7 +7,8 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Recommendations" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Summary" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,15 +442,20 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Recommended_Assessment_Name</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>Recommended_Assessment</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Similarity_Score</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Explanation</t>
         </is>
@@ -457,66 +463,6 @@
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
-        <is>
-          <t>Looking to hire mid-level professionals who are proficient in Python, SQL and Java Script. Need an assessment package that can test all skills with max duration of 60 minutes.</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>https://www.shl.com/solutions/products/product-catalog/view/automata-fix-new/</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>0.335</v>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Matched due to overlap in key terms: java, can, an, looking, assessment, that, minutes, with, in, who</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Looking to hire mid-level professionals who are proficient in Python, SQL and Java Script. Need an assessment package that can test all skills with max duration of 60 minutes.</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>https://www.shl.com/solutions/products/product-catalog/view/core-java-entry-level-new/</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>0.335</v>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Matched due to overlap in key terms: java, can, an, looking, assessment, that, minutes, with, in, who</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Looking to hire mid-level professionals who are proficient in Python, SQL and Java Script. Need an assessment package that can test all skills with max duration of 60 minutes.</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>https://www.shl.com/solutions/products/product-catalog/view/java-8-new/</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>0.335</v>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Matched due to overlap in key terms: java, can, an, looking, assessment, that, minutes, with, in, who</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
         <is>
           <t>Job Description
  Join a community that is shaping the future of work! 
@@ -559,22 +505,27 @@
 Can you recommend some assessment that can help me screen applications. Time limit is less than 30 minutes</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Javascript New</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
         <is>
           <t>https://www.shl.com/solutions/products/product-catalog/view/javascript-new/</t>
         </is>
       </c>
-      <c r="C5" t="n">
-        <v>0.89</v>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Matched due to overlap in key terms: insight, looking, science, huge, flexibility, market, ago, candidates, key, best, develop, touch, lead, diversity, workplace, sure, find, excellent, through, business, with, lifeatshl, careeropportunities, than, no, success, years, family, coaching, job, one, is, ability, services, future, around, an, shlhiringtalent, s, solution, transform, talent, are, knowledgeable, description, how, to, become, contribute, experience, us, flexible, careersatshl, fabric, join, workplaces, as, development, encourage, world, inclusion, breaking, something, engineer, me, started, adjustments, possible, career, ongoing, you, your, out, at, about, takes, there, we, goals, inclusivity, employer, shl, when, industry, offer, the, businesses, growth, and, experiences, time, guidance, process, jobopportunities, knowledge, others, shaping, possibilities, from, opportunity, unlock, insights, fun, equity, accessibility, that, power, threads, choose, desirable, more, product, doing, care, technology, get, this, greatest, inspired, continue, products, path, new, people, so, help, by, make, equal, 40, where, culture, scale, be, community, work, offered, assessment, transformational, lives, will, intrinsic, off, making, in, collaboration, acquisition, outcomes, team, package, employee, achieve, application, do, all, better, friendly, benefits, ll, manager, launches, what, on, transformation, ground, a, investment, dei, for, applications, answers, can, part, support, inclusive, essential, inspire, of, range, recruitment, our, diverse, currently, powerhouse</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
+      <c r="D2" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Recommended because the job description shares key focus areas such as 40, range, contribute, investment, adjustments, application, outcomes, transformation, desirable, future, culture, shlhiringtalent, and, in, help, workplace, lead, can, with, breaking, for, product, doing, years, employee, scale, sure, your, assessment, all, community, path, greatest, goals, possible, friendly, benefits, candidates, achieve, package, the, people, threads, more, part, excellent, currently, job, market, business, touch, power, ability, is, description, me, are, time, world, growth, an, when, accessibility, coaching, better, develop, flexibility, huge, how, acquisition, than, ongoing, guidance, this, our, on, started, dei, support, become, success, at, shl, flexible, ll, transform, experience, looking, find, out, ago, of, work, ground, inclusivity, essential, unlock, we, possibilities, choose, continue, what, key, there, lifeatshl, shaping, you, off, fabric, get, one, recruitment, businesses, careeropportunities, join, offered, career, from, diversity, intrinsic, careersatshl, talent, something, technology, insights, do, by, industry, jobopportunities, inspire, transformational, experiences, no, diverse, inspired, insight, s, family, team, that, collaboration, products, knowledge, through, powerhouse, inclusive, about, services, development, engineer, make, where, knowledgeable, inclusion, others, so, opportunity, making, us, care, launches, a, will, encourage, employer, manager, takes, solution, lives, as, offer, new, equity, best, applications, science, process, around, answers, equal, be, workplaces, fun, to</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
         <is>
           <t>Job Description
  Join a community that is shaping the future of work! 
@@ -617,22 +568,27 @@
 Can you recommend some assessment that can help me screen applications. Time limit is less than 30 minutes</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>https://www.shl.com/solutions/products/product-catalog/view/automata-selenium/</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>0.89</v>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Matched due to overlap in key terms: insight, looking, science, huge, flexibility, market, ago, candidates, key, best, develop, touch, lead, diversity, workplace, sure, find, excellent, through, business, with, lifeatshl, careeropportunities, than, no, success, years, family, coaching, job, one, is, ability, services, future, around, an, shlhiringtalent, s, solution, transform, talent, are, knowledgeable, description, how, to, become, contribute, experience, us, flexible, careersatshl, fabric, join, workplaces, as, development, encourage, world, inclusion, breaking, something, engineer, me, started, adjustments, possible, career, ongoing, you, your, out, at, about, takes, there, we, goals, inclusivity, employer, shl, when, industry, offer, the, businesses, growth, and, experiences, time, guidance, process, jobopportunities, knowledge, others, shaping, possibilities, from, opportunity, unlock, insights, fun, equity, accessibility, that, power, threads, choose, desirable, more, product, doing, care, technology, get, this, greatest, inspired, continue, products, path, new, people, so, help, by, make, equal, 40, where, culture, scale, be, community, work, offered, assessment, transformational, lives, will, intrinsic, off, making, in, collaboration, acquisition, outcomes, team, package, employee, achieve, application, do, all, better, friendly, benefits, ll, manager, launches, what, on, transformation, ground, a, investment, dei, for, applications, answers, can, part, support, inclusive, essential, inspire, of, range, recruitment, our, diverse, currently, powerhouse</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Sql Server New</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>https://www.shl.com/solutions/products/product-catalog/view/sql-server-new/</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Recommended because the job description shares key focus areas such as 40, range, contribute, investment, adjustments, application, outcomes, transformation, desirable, future, culture, shlhiringtalent, and, in, help, workplace, lead, can, with, breaking, for, product, doing, years, employee, scale, sure, your, assessment, all, community, path, greatest, goals, possible, friendly, benefits, candidates, achieve, package, the, people, threads, more, part, excellent, currently, job, market, business, touch, power, ability, is, description, me, are, time, world, growth, an, when, accessibility, coaching, better, develop, flexibility, huge, how, acquisition, than, ongoing, guidance, this, our, on, started, dei, support, become, success, at, shl, flexible, ll, transform, experience, looking, find, out, ago, of, work, ground, inclusivity, essential, unlock, we, possibilities, choose, continue, what, key, there, lifeatshl, shaping, you, off, fabric, get, one, recruitment, businesses, careeropportunities, join, offered, career, from, diversity, intrinsic, careersatshl, talent, something, technology, insights, do, by, industry, jobopportunities, inspire, transformational, experiences, no, diverse, inspired, insight, s, family, team, that, collaboration, products, knowledge, through, powerhouse, inclusive, about, services, development, engineer, make, where, knowledgeable, inclusion, others, so, opportunity, making, us, care, launches, a, will, encourage, employer, manager, takes, solution, lives, as, offer, new, equity, best, applications, science, process, around, answers, equal, be, workplaces, fun, to</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
         <is>
           <t>Job Description
  Join a community that is shaping the future of work! 
@@ -675,82 +631,27 @@
 Can you recommend some assessment that can help me screen applications. Time limit is less than 30 minutes</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>https://www.shl.com/products/product-catalog/view/professional-7-1-solution/</t>
-        </is>
-      </c>
-      <c r="C7" t="n">
-        <v>0.89</v>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>Matched due to overlap in key terms: insight, looking, science, huge, flexibility, market, ago, candidates, key, best, develop, touch, lead, diversity, workplace, sure, find, excellent, through, business, with, lifeatshl, careeropportunities, than, no, success, years, family, coaching, job, one, is, ability, services, future, around, an, shlhiringtalent, s, solution, transform, talent, are, knowledgeable, description, how, to, become, contribute, experience, us, flexible, careersatshl, fabric, join, workplaces, as, development, encourage, world, inclusion, breaking, something, engineer, me, started, adjustments, possible, career, ongoing, you, your, out, at, about, takes, there, we, goals, inclusivity, employer, shl, when, industry, offer, the, businesses, growth, and, experiences, time, guidance, process, jobopportunities, knowledge, others, shaping, possibilities, from, opportunity, unlock, insights, fun, equity, accessibility, that, power, threads, choose, desirable, more, product, doing, care, technology, get, this, greatest, inspired, continue, products, path, new, people, so, help, by, make, equal, 40, where, culture, scale, be, community, work, offered, assessment, transformational, lives, will, intrinsic, off, making, in, collaboration, acquisition, outcomes, team, package, employee, achieve, application, do, all, better, friendly, benefits, ll, manager, launches, what, on, transformation, ground, a, investment, dei, for, applications, answers, can, part, support, inclusive, essential, inspire, of, range, recruitment, our, diverse, currently, powerhouse</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>I am hiring for an analyst and wants applications to screen using Cognitive and personality tests, what options are available within 45 mins.</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>https://www.shl.com/solutions/products/product-catalog/view/javascript-new/</t>
-        </is>
-      </c>
-      <c r="C8" t="n">
-        <v>0.244</v>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>Matched due to overlap in key terms: what, applications, an, and, are, to, for, tests</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>I am hiring for an analyst and wants applications to screen using Cognitive and personality tests, what options are available within 45 mins.</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Manual Testing New</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
         <is>
           <t>https://www.shl.com/solutions/products/product-catalog/view/manual-testing-new/</t>
         </is>
       </c>
-      <c r="C9" t="n">
-        <v>0.244</v>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>Matched due to overlap in key terms: what, applications, an, and, are, to, for, tests</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>I am hiring for an analyst and wants applications to screen using Cognitive and personality tests, what options are available within 45 mins.</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>https://www.shl.com/solutions/products/product-catalog/view/automata-selenium/</t>
-        </is>
-      </c>
-      <c r="C10" t="n">
-        <v>0.244</v>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>Matched due to overlap in key terms: what, applications, an, and, are, to, for, tests</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
+      <c r="D4" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Recommended because the job description shares key focus areas such as 40, range, contribute, investment, adjustments, application, outcomes, transformation, desirable, future, culture, shlhiringtalent, and, in, help, workplace, lead, can, with, breaking, for, product, doing, years, employee, scale, sure, your, assessment, all, community, path, greatest, goals, possible, friendly, benefits, candidates, achieve, package, the, people, threads, more, part, excellent, currently, job, market, business, touch, power, ability, is, description, me, are, time, world, growth, an, when, accessibility, coaching, better, develop, flexibility, huge, how, acquisition, than, ongoing, guidance, this, our, on, started, dei, support, become, success, at, shl, flexible, ll, transform, experience, looking, find, out, ago, of, work, ground, inclusivity, essential, unlock, we, possibilities, choose, continue, what, key, there, lifeatshl, shaping, you, off, fabric, get, one, recruitment, businesses, careeropportunities, join, offered, career, from, diversity, intrinsic, careersatshl, talent, something, technology, insights, do, by, industry, jobopportunities, inspire, transformational, experiences, no, diverse, inspired, insight, s, family, team, that, collaboration, products, knowledge, through, powerhouse, inclusive, about, services, development, engineer, make, where, knowledgeable, inclusion, others, so, opportunity, making, us, care, launches, a, will, encourage, employer, manager, takes, solution, lives, as, offer, new, equity, best, applications, science, process, around, answers, equal, be, workplaces, fun, to</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
         <is>
           <t>I have a JD Job Description
  People Science. People Answers  !
@@ -814,22 +715,27 @@
 Here and I have want them to give a test which is atleast  30 mins long</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Javascript New</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
         <is>
           <t>https://www.shl.com/solutions/products/product-catalog/view/javascript-new/</t>
         </is>
       </c>
-      <c r="C11" t="n">
-        <v>0.771</v>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>Matched due to overlap in key terms: insight, science, want, huge, flexibility, market, ago, candidates, key, best, develop, touch, lead, diversity, design, workplace, sure, find, excellent, through, business, with, lifeatshl, than, no, success, years, family, coaching, job, or, one, is, ability, services, around, an, s, solution, transform, talent, are, knowledgeable, description, how, to, become, experience, us, flexible, careersatshl, fabric, join, workplaces, as, development, encourage, world, inclusion, breaking, something, started, getting, adjustments, possible, career, ongoing, you, your, out, at, ready, about, takes, there, we, goals, inclusivity, employer, shl, when, industry, offer, the, businesses, growth, and, required, experiences, time, guidance, process, knowledge, others, possibilities, test, from, opportunity, unlock, quality, insights, fun, equity, accessibility, that, solutions, power, threads, choose, desirable, more, product, care, technology, get, this, greatest, inspired, continue, products, path, new, people, so, help, by, make, equal, functional, 40, where, culture, scale, be, work, offered, transformational, lives, will, intrinsic, off, making, in, collaboration, acquisition, create, team, package, outcomes, employee, achieve, application, do, all, better, benefits, ll, manager, launches, what, on, transformation, ground, a, investment, dei, long, for, applications, answers, can, part, support, inclusive, inspire, creating, strong, of, range, recruitment, our, diverse, currently, powerhouse</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
+      <c r="D5" t="n">
+        <v>0.5620000000000001</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Recommended because the job description shares key focus areas such as 40, range, investment, adjustments, application, outcomes, transformation, desirable, culture, and, in, long, help, workplace, lead, can, with, breaking, want, for, product, years, employee, scale, sure, required, your, creating, all, solutions, path, greatest, goals, possible, benefits, create, candidates, achieve, package, the, people, threads, more, part, strong, excellent, currently, job, market, business, touch, power, ability, is, description, world, are, time, growth, an, when, accessibility, coaching, better, ready, develop, design, flexibility, huge, how, acquisition, than, ongoing, guidance, this, our, on, started, dei, support, become, success, at, shl, flexible, ll, transform, experience, find, out, ago, of, work, ground, inclusivity, possibilities, unlock, we, continue, choose, key, what, there, lifeatshl, you, off, fabric, get, one, recruitment, businesses, join, offered, career, from, diversity, intrinsic, careersatshl, functional, talent, something, technology, insights, do, by, industry, or, inspire, transformational, experiences, no, diverse, inspired, insight, s, family, team, that, collaboration, products, quality, knowledge, through, powerhouse, inclusive, about, services, development, make, where, knowledgeable, inclusion, others, so, opportunity, making, us, care, test, launches, a, will, encourage, employer, manager, takes, solution, lives, as, offer, new, equity, getting, best, science, applications, around, process, answers, equal, be, workplaces, fun, to</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
         <is>
           <t>I have a JD Job Description
  People Science. People Answers  !
@@ -893,22 +799,27 @@
 Here and I have want them to give a test which is atleast  30 mins long</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Professional 7 1 Solution</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
         <is>
           <t>https://www.shl.com/products/product-catalog/view/professional-7-1-solution/</t>
         </is>
       </c>
-      <c r="C12" t="n">
-        <v>0.771</v>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>Matched due to overlap in key terms: insight, science, want, huge, flexibility, market, ago, candidates, key, best, develop, touch, lead, diversity, design, workplace, sure, find, excellent, through, business, with, lifeatshl, than, no, success, years, family, coaching, job, or, one, is, ability, services, around, an, s, solution, transform, talent, are, knowledgeable, description, how, to, become, experience, us, flexible, careersatshl, fabric, join, workplaces, as, development, encourage, world, inclusion, breaking, something, started, getting, adjustments, possible, career, ongoing, you, your, out, at, ready, about, takes, there, we, goals, inclusivity, employer, shl, when, industry, offer, the, businesses, growth, and, required, experiences, time, guidance, process, knowledge, others, possibilities, test, from, opportunity, unlock, quality, insights, fun, equity, accessibility, that, solutions, power, threads, choose, desirable, more, product, care, technology, get, this, greatest, inspired, continue, products, path, new, people, so, help, by, make, equal, functional, 40, where, culture, scale, be, work, offered, transformational, lives, will, intrinsic, off, making, in, collaboration, acquisition, create, team, package, outcomes, employee, achieve, application, do, all, better, benefits, ll, manager, launches, what, on, transformation, ground, a, investment, dei, long, for, applications, answers, can, part, support, inclusive, inspire, creating, strong, of, range, recruitment, our, diverse, currently, powerhouse</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
+      <c r="D6" t="n">
+        <v>0.5620000000000001</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Recommended because the job description shares key focus areas such as 40, range, investment, adjustments, application, outcomes, transformation, desirable, culture, and, in, long, help, workplace, lead, can, with, breaking, want, for, product, years, employee, scale, sure, required, your, creating, all, solutions, path, greatest, goals, possible, benefits, create, candidates, achieve, package, the, people, threads, more, part, strong, excellent, currently, job, market, business, touch, power, ability, is, description, world, are, time, growth, an, when, accessibility, coaching, better, ready, develop, design, flexibility, huge, how, acquisition, than, ongoing, guidance, this, our, on, started, dei, support, become, success, at, shl, flexible, ll, transform, experience, find, out, ago, of, work, ground, inclusivity, possibilities, unlock, we, continue, choose, key, what, there, lifeatshl, you, off, fabric, get, one, recruitment, businesses, join, offered, career, from, diversity, intrinsic, careersatshl, functional, talent, something, technology, insights, do, by, industry, or, inspire, transformational, experiences, no, diverse, inspired, insight, s, family, team, that, collaboration, products, quality, knowledge, through, powerhouse, inclusive, about, services, development, make, where, knowledgeable, inclusion, others, so, opportunity, making, us, care, test, launches, a, will, encourage, employer, manager, takes, solution, lives, as, offer, new, equity, getting, best, science, applications, around, process, answers, equal, be, workplaces, fun, to</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
         <is>
           <t>I have a JD Job Description
  People Science. People Answers  !
@@ -972,244 +883,177 @@
 Here and I have want them to give a test which is atleast  30 mins long</t>
         </is>
       </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Htmlcss New</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>https://www.shl.com/solutions/products/product-catalog/view/htmlcss-new/</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>0.5620000000000001</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Recommended because the job description shares key focus areas such as 40, range, investment, adjustments, application, outcomes, transformation, desirable, culture, and, in, long, help, workplace, lead, can, with, breaking, want, for, product, years, employee, scale, sure, required, your, creating, all, solutions, path, greatest, goals, possible, benefits, create, candidates, achieve, package, the, people, threads, more, part, strong, excellent, currently, job, market, business, touch, power, ability, is, description, world, are, time, growth, an, when, accessibility, coaching, better, ready, develop, design, flexibility, huge, how, acquisition, than, ongoing, guidance, this, our, on, started, dei, support, become, success, at, shl, flexible, ll, transform, experience, find, out, ago, of, work, ground, inclusivity, possibilities, unlock, we, continue, choose, key, what, there, lifeatshl, you, off, fabric, get, one, recruitment, businesses, join, offered, career, from, diversity, intrinsic, careersatshl, functional, talent, something, technology, insights, do, by, industry, or, inspire, transformational, experiences, no, diverse, inspired, insight, s, family, team, that, collaboration, products, quality, knowledge, through, powerhouse, inclusive, about, services, development, make, where, knowledgeable, inclusion, others, so, opportunity, making, us, care, test, launches, a, will, encourage, employer, manager, takes, solution, lives, as, offer, new, equity, getting, best, science, applications, around, process, answers, equal, be, workplaces, fun, to</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>I am new looking for new graduates in my sales team, suggest an 30 min long assessment</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Interpersonal Communications</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>https://www.shl.com/products/product-catalog/view/interpersonal-communications/</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>0.331</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Recommended because the job description shares key focus areas such as my, for, sales, new, i, in, an, graduates</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>I am new looking for new graduates in my sales team, suggest an 30 min long assessment</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Svar Spoken English Indian Accent New</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>https://www.shl.com/solutions/products/product-catalog/view/svar-spoken-english-indian-accent-new/</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>0.331</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Recommended because the job description shares key focus areas such as my, for, sales, new, i, in, an, graduates</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>I am new looking for new graduates in my sales team, suggest an 30 min long assessment</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Technical Sales Associate Solution</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>https://www.shl.com/solutions/products/product-catalog/view/technical-sales-associate-solution/</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>0.331</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Recommended because the job description shares key focus areas such as my, for, sales, new, i, in, an, graduates</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>I want to hire a product manager with 3-4 years of work experience and expertise in SDLC, Jira and Confluence</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Data Warehousing Concepts</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>https://www.shl.com/solutions/products/product-catalog/view/data-warehousing-concepts/</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>0.312</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Recommended because the job description shares key focus areas such as with, and, want, hire, expertise, a, i, in, experience, years, of, to</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>I want to hire a product manager with 3-4 years of work experience and expertise in SDLC, Jira and Confluence</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Professional 7 0 Solution 3958</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>https://www.shl.com/solutions/products/product-catalog/view/professional-7-0-solution-3958/</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>0.312</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Recommended because the job description shares key focus areas such as with, and, want, hire, expertise, a, i, in, experience, years, of, to</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>I want to hire a product manager with 3-4 years of work experience and expertise in SDLC, Jira and Confluence</t>
+        </is>
+      </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>https://www.shl.com/solutions/products/product-catalog/view/sql-server-new/</t>
-        </is>
-      </c>
-      <c r="C13" t="n">
-        <v>0.771</v>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>Matched due to overlap in key terms: insight, science, want, huge, flexibility, market, ago, candidates, key, best, develop, touch, lead, diversity, design, workplace, sure, find, excellent, through, business, with, lifeatshl, than, no, success, years, family, coaching, job, or, one, is, ability, services, around, an, s, solution, transform, talent, are, knowledgeable, description, how, to, become, experience, us, flexible, careersatshl, fabric, join, workplaces, as, development, encourage, world, inclusion, breaking, something, started, getting, adjustments, possible, career, ongoing, you, your, out, at, ready, about, takes, there, we, goals, inclusivity, employer, shl, when, industry, offer, the, businesses, growth, and, required, experiences, time, guidance, process, knowledge, others, possibilities, test, from, opportunity, unlock, quality, insights, fun, equity, accessibility, that, solutions, power, threads, choose, desirable, more, product, care, technology, get, this, greatest, inspired, continue, products, path, new, people, so, help, by, make, equal, functional, 40, where, culture, scale, be, work, offered, transformational, lives, will, intrinsic, off, making, in, collaboration, acquisition, create, team, package, outcomes, employee, achieve, application, do, all, better, benefits, ll, manager, launches, what, on, transformation, ground, a, investment, dei, long, for, applications, answers, can, part, support, inclusive, inspire, creating, strong, of, range, recruitment, our, diverse, currently, powerhouse</t>
+          <t>Microsoft Excel 365 Essentials New</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>https://www.shl.com/solutions/products/product-catalog/view/microsoft-excel-365-essentials-new/</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>0.312</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Recommended because the job description shares key focus areas such as with, and, want, hire, expertise, a, i, in, experience, years, of, to</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
-        <is>
-          <t>I am new looking for new graduates in my sales team, suggest an 30 min long assessment</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>https://www.shl.com/products/product-catalog/view/interpersonal-communications/</t>
-        </is>
-      </c>
-      <c r="C14" t="n">
-        <v>0.335</v>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>Matched due to overlap in key terms: an, new, graduates, i, sales, in, for, my</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>I am new looking for new graduates in my sales team, suggest an 30 min long assessment</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>https://www.shl.com/solutions/products/product-catalog/view/english-comprehension-new/</t>
-        </is>
-      </c>
-      <c r="C15" t="n">
-        <v>0.335</v>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>Matched due to overlap in key terms: an, new, graduates, i, sales, in, for, my</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>I am new looking for new graduates in my sales team, suggest an 30 min long assessment</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>https://www.shl.com/solutions/products/product-catalog/view/entry-level-sales-7-1/</t>
-        </is>
-      </c>
-      <c r="C16" t="n">
-        <v>0.335</v>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>Matched due to overlap in key terms: an, new, graduates, i, sales, in, for, my</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>For Marketing - Content Writer Position
-Department: Marketing
-Location: Gurugram
-About Company
-ShopClues.com is India's leading e-commerce platform that is focused on changing the shopping scenario of the country. We are the one-stop platform for everything from electronics to fashion to home &amp; kitchen. The company visions to be the largest and most customer-centric e-commerce platform for India.
-ShopClues.com has been operating out of Silicon Valley since February 2011 and has its headquarters in Gurugram. The Company launched its Beta version on 26th January 2012 and has been constantly evolving since then for the better.
-Our Culture
-We are a team of enthusiastic and determined individuals, who believe in working together with lots of energy, bringing continuous innovations to the organization, and celebrating every bit of it. We provide equal opportunity to each individual and look forward to executing the best ideas.
-The Typical Creative Process Involves
-Discussing the campaign's core message and target audience
-Brainstorming visual and copy ideas with other members of the creative team
-Visualizing different forms of communication approaches for various marketing platforms like Website, Email, Social, etc. for ShopClues.
-Generating Stories for Brands core blog, and other content-driven platforms.
-Overseeing the production phase till the final output.
-Experience in the publishing of Push Notification and unique Product Description.</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>https://www.shl.com/solutions/products/product-catalog/view/verify-verbal-ability-next-generation/</t>
-        </is>
-      </c>
-      <c r="C17" t="n">
-        <v>0.463</v>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>Matched due to overlap in key terms: other, culture, be, content, best, opportunity, in, e, team, working, driven, that, continuous, with, about, on, we, provide, organization, communication, product, a, members, individuals, one, is, the, for, com, leading, s, and, are, description, of, to, executing, equal, experience, position</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>For Marketing - Content Writer Position
-Department: Marketing
-Location: Gurugram
-About Company
-ShopClues.com is India's leading e-commerce platform that is focused on changing the shopping scenario of the country. We are the one-stop platform for everything from electronics to fashion to home &amp; kitchen. The company visions to be the largest and most customer-centric e-commerce platform for India.
-ShopClues.com has been operating out of Silicon Valley since February 2011 and has its headquarters in Gurugram. The Company launched its Beta version on 26th January 2012 and has been constantly evolving since then for the better.
-Our Culture
-We are a team of enthusiastic and determined individuals, who believe in working together with lots of energy, bringing continuous innovations to the organization, and celebrating every bit of it. We provide equal opportunity to each individual and look forward to executing the best ideas.
-The Typical Creative Process Involves
-Discussing the campaign's core message and target audience
-Brainstorming visual and copy ideas with other members of the creative team
-Visualizing different forms of communication approaches for various marketing platforms like Website, Email, Social, etc. for ShopClues.
-Generating Stories for Brands core blog, and other content-driven platforms.
-Overseeing the production phase till the final output.
-Experience in the publishing of Push Notification and unique Product Description.</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>https://www.shl.com/solutions/products/product-catalog/view/professional-7-1-solution/</t>
-        </is>
-      </c>
-      <c r="C18" t="n">
-        <v>0.463</v>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>Matched due to overlap in key terms: other, culture, be, content, best, opportunity, in, e, team, working, driven, that, continuous, with, about, on, we, provide, organization, communication, product, a, members, individuals, one, is, the, for, com, leading, s, and, are, description, of, to, executing, equal, experience, position</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>For Marketing - Content Writer Position
-Department: Marketing
-Location: Gurugram
-About Company
-ShopClues.com is India's leading e-commerce platform that is focused on changing the shopping scenario of the country. We are the one-stop platform for everything from electronics to fashion to home &amp; kitchen. The company visions to be the largest and most customer-centric e-commerce platform for India.
-ShopClues.com has been operating out of Silicon Valley since February 2011 and has its headquarters in Gurugram. The Company launched its Beta version on 26th January 2012 and has been constantly evolving since then for the better.
-Our Culture
-We are a team of enthusiastic and determined individuals, who believe in working together with lots of energy, bringing continuous innovations to the organization, and celebrating every bit of it. We provide equal opportunity to each individual and look forward to executing the best ideas.
-The Typical Creative Process Involves
-Discussing the campaign's core message and target audience
-Brainstorming visual and copy ideas with other members of the creative team
-Visualizing different forms of communication approaches for various marketing platforms like Website, Email, Social, etc. for ShopClues.
-Generating Stories for Brands core blog, and other content-driven platforms.
-Overseeing the production phase till the final output.
-Experience in the publishing of Push Notification and unique Product Description.</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>https://www.shl.com/solutions/products/product-catalog/view/shl-verify-interactive-numerical-calculation/</t>
-        </is>
-      </c>
-      <c r="C19" t="n">
-        <v>0.463</v>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>Matched due to overlap in key terms: other, culture, be, content, best, opportunity, in, e, team, working, driven, that, continuous, with, about, on, we, provide, organization, communication, product, a, members, individuals, one, is, the, for, com, leading, s, and, are, description, of, to, executing, equal, experience, position</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>I want to hire a product manager with 3-4 years of work experience and expertise in SDLC, Jira and Confluence</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>https://www.shl.com/solutions/products/product-catalog/view/data-warehousing-concepts/</t>
-        </is>
-      </c>
-      <c r="C20" t="n">
-        <v>0.495</v>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>Matched due to overlap in key terms: and, want, expertise, a, years, i, hire, of, to, with, experience, in</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>I want to hire a product manager with 3-4 years of work experience and expertise in SDLC, Jira and Confluence</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>https://www.shl.com/solutions/products/product-catalog/view/professional-7-0-solution-3958/</t>
-        </is>
-      </c>
-      <c r="C21" t="n">
-        <v>0.495</v>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>Matched due to overlap in key terms: and, want, expertise, a, years, i, hire, of, to, with, experience, in</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>I want to hire a product manager with 3-4 years of work experience and expertise in SDLC, Jira and Confluence</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>https://www.shl.com/solutions/products/product-catalog/view/microsoft-excel-365-essentials-new/</t>
-        </is>
-      </c>
-      <c r="C22" t="n">
-        <v>0.495</v>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>Matched due to overlap in key terms: and, want, expertise, a, years, i, hire, of, to, with, experience, in</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
         <is>
           <t>Suggest me an assessment for the JD below Job Description
  Find purpose in each day while contributing to a workplace revolution! SHL, People Science. People Answers. 
@@ -1248,22 +1092,27 @@
 SHL is an equal opportunity employer. We support and encourage applications from a diverse range of candidates. We can, and do make adjustments to make sure our recruitment process is as inclusive as possible.</t>
         </is>
       </c>
-      <c r="B23" t="inlineStr">
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Javascript New</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
         <is>
           <t>https://www.shl.com/solutions/products/product-catalog/view/javascript-new/</t>
         </is>
       </c>
-      <c r="C23" t="n">
-        <v>0.834</v>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>Matched due to overlap in key terms: insight, looking, science, huge, flexibility, market, ago, candidates, key, best, develop, touch, lead, diversity, workplace, sure, find, excellent, through, business, with, lifeatshl, management, than, no, success, years, family, coaching, job, or, one, is, ability, services, around, an, shlhiringtalent, s, transform, talent, are, knowledgeable, description, how, to, become, experience, below, us, flexible, careersatshl, fabric, join, workplaces, as, development, encourage, world, inclusion, breaking, something, me, started, adjustments, possible, career, ongoing, you, your, out, at, about, takes, there, we, providing, goals, inclusivity, employer, shl, when, industry, offer, the, businesses, growth, and, experiences, time, guidance, process, knowledge, others, possibilities, 1, from, opportunity, unlock, quality, insights, fun, equity, accessibility, that, power, processes, threads, choose, more, product, doing, care, technology, get, this, greatest, inspired, continue, products, path, new, people, so, help, by, make, equal, 40, where, culture, scale, be, work, offered, assessment, transformational, lives, will, intrinsic, off, making, in, collaboration, acquisition, outcomes, team, package, employee, achieve, application, do, all, better, friendly, benefits, ll, manager, launches, what, on, transformation, ground, a, investment, dei, for, applications, answers, can, part, support, inclusive, inspire, strong, of, range, recruitment, our, diverse, currently, powerhouse</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
+      <c r="D14" t="n">
+        <v>0.663</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Recommended because the job description shares key focus areas such as 40, range, investment, adjustments, application, outcomes, transformation, culture, shlhiringtalent, and, in, help, workplace, lead, can, with, breaking, for, product, doing, management, years, providing, scale, employee, sure, processes, your, assessment, all, path, greatest, goals, possible, friendly, benefits, candidates, achieve, package, the, people, threads, more, part, strong, excellent, currently, job, market, business, touch, power, ability, is, description, me, are, time, world, growth, an, when, accessibility, coaching, better, develop, flexibility, huge, how, below, acquisition, than, ongoing, guidance, this, our, on, started, dei, support, become, success, at, shl, flexible, ll, transform, experience, looking, find, out, ago, of, work, ground, inclusivity, possibilities, unlock, we, continue, choose, key, what, there, lifeatshl, you, off, fabric, get, one, recruitment, businesses, join, offered, career, from, diversity, intrinsic, careersatshl, talent, something, technology, insights, do, by, industry, or, inspire, transformational, experiences, no, diverse, inspired, insight, s, family, team, 1, that, collaboration, products, quality, knowledge, through, powerhouse, inclusive, about, services, development, make, where, knowledgeable, inclusion, others, so, opportunity, making, us, care, launches, a, will, encourage, employer, manager, takes, lives, as, offer, new, equity, best, applications, science, process, around, answers, equal, be, workplaces, fun, to</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
         <is>
           <t>Suggest me an assessment for the JD below Job Description
  Find purpose in each day while contributing to a workplace revolution! SHL, People Science. People Answers. 
@@ -1302,22 +1151,27 @@
 SHL is an equal opportunity employer. We support and encourage applications from a diverse range of candidates. We can, and do make adjustments to make sure our recruitment process is as inclusive as possible.</t>
         </is>
       </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>https://www.shl.com/solutions/products/product-catalog/view/automata-selenium/</t>
-        </is>
-      </c>
-      <c r="C24" t="n">
-        <v>0.834</v>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>Matched due to overlap in key terms: insight, looking, science, huge, flexibility, market, ago, candidates, key, best, develop, touch, lead, diversity, workplace, sure, find, excellent, through, business, with, lifeatshl, management, than, no, success, years, family, coaching, job, or, one, is, ability, services, around, an, shlhiringtalent, s, transform, talent, are, knowledgeable, description, how, to, become, experience, below, us, flexible, careersatshl, fabric, join, workplaces, as, development, encourage, world, inclusion, breaking, something, me, started, adjustments, possible, career, ongoing, you, your, out, at, about, takes, there, we, providing, goals, inclusivity, employer, shl, when, industry, offer, the, businesses, growth, and, experiences, time, guidance, process, knowledge, others, possibilities, 1, from, opportunity, unlock, quality, insights, fun, equity, accessibility, that, power, processes, threads, choose, more, product, doing, care, technology, get, this, greatest, inspired, continue, products, path, new, people, so, help, by, make, equal, 40, where, culture, scale, be, work, offered, assessment, transformational, lives, will, intrinsic, off, making, in, collaboration, acquisition, outcomes, team, package, employee, achieve, application, do, all, better, friendly, benefits, ll, manager, launches, what, on, transformation, ground, a, investment, dei, for, applications, answers, can, part, support, inclusive, inspire, strong, of, range, recruitment, our, diverse, currently, powerhouse</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Professional 7 1 Solution</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>https://www.shl.com/products/product-catalog/view/professional-7-1-solution/</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>0.663</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Recommended because the job description shares key focus areas such as 40, range, investment, adjustments, application, outcomes, transformation, culture, shlhiringtalent, and, in, help, workplace, lead, can, with, breaking, for, product, doing, management, years, providing, scale, employee, sure, processes, your, assessment, all, path, greatest, goals, possible, friendly, benefits, candidates, achieve, package, the, people, threads, more, part, strong, excellent, currently, job, market, business, touch, power, ability, is, description, me, are, time, world, growth, an, when, accessibility, coaching, better, develop, flexibility, huge, how, below, acquisition, than, ongoing, guidance, this, our, on, started, dei, support, become, success, at, shl, flexible, ll, transform, experience, looking, find, out, ago, of, work, ground, inclusivity, possibilities, unlock, we, continue, choose, key, what, there, lifeatshl, you, off, fabric, get, one, recruitment, businesses, join, offered, career, from, diversity, intrinsic, careersatshl, talent, something, technology, insights, do, by, industry, or, inspire, transformational, experiences, no, diverse, inspired, insight, s, family, team, 1, that, collaboration, products, quality, knowledge, through, powerhouse, inclusive, about, services, development, make, where, knowledgeable, inclusion, others, so, opportunity, making, us, care, launches, a, will, encourage, employer, manager, takes, lives, as, offer, new, equity, best, applications, science, process, around, answers, equal, be, workplaces, fun, to</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
         <is>
           <t>Suggest me an assessment for the JD below Job Description
  Find purpose in each day while contributing to a workplace revolution! SHL, People Science. People Answers. 
@@ -1356,171 +1210,84 @@
 SHL is an equal opportunity employer. We support and encourage applications from a diverse range of candidates. We can, and do make adjustments to make sure our recruitment process is as inclusive as possible.</t>
         </is>
       </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>https://www.shl.com/products/product-catalog/view/professional-7-1-solution/</t>
-        </is>
-      </c>
-      <c r="C25" t="n">
-        <v>0.834</v>
-      </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>Matched due to overlap in key terms: insight, looking, science, huge, flexibility, market, ago, candidates, key, best, develop, touch, lead, diversity, workplace, sure, find, excellent, through, business, with, lifeatshl, management, than, no, success, years, family, coaching, job, or, one, is, ability, services, around, an, shlhiringtalent, s, transform, talent, are, knowledgeable, description, how, to, become, experience, below, us, flexible, careersatshl, fabric, join, workplaces, as, development, encourage, world, inclusion, breaking, something, me, started, adjustments, possible, career, ongoing, you, your, out, at, about, takes, there, we, providing, goals, inclusivity, employer, shl, when, industry, offer, the, businesses, growth, and, experiences, time, guidance, process, knowledge, others, possibilities, 1, from, opportunity, unlock, quality, insights, fun, equity, accessibility, that, power, processes, threads, choose, more, product, doing, care, technology, get, this, greatest, inspired, continue, products, path, new, people, so, help, by, make, equal, 40, where, culture, scale, be, work, offered, assessment, transformational, lives, will, intrinsic, off, making, in, collaboration, acquisition, outcomes, team, package, employee, achieve, application, do, all, better, friendly, benefits, ll, manager, launches, what, on, transformation, ground, a, investment, dei, for, applications, answers, can, part, support, inclusive, inspire, strong, of, range, recruitment, our, diverse, currently, powerhouse</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>I want to hire Customer support executives who are expert in English communication.  
-We are looking for talented Customer Support specialists to join our Product operations team in India (Mumbai)
-Minna connects global banks and fintech with subscription businesses to give consumers self-serve subscription management in-app. Minna is a technology partner to top-tier financial institutions, fintech and subscription businesses, providing subscription management functionality for 50+ million banking and fintech customers across the United States, United Kingdom and Europe.
-Minna builds the infrastructure that links Subscription Merchants (such as Netflix, Spotify, Amazon) to leading Financial Institutions (Lloyds Bank, ING Belgium, Swedbank to name a few). This connection enables consumers to effortlessly manage their subscriptions by performing actions like canceling, pausing, or changing their plans.
-Responsibilities:
-Efficiently manage cancellations and monitor cancellation status for merchants
-Initiate and execute workflows for cancellations at various stages of the cancellation journey with merchants
-Provide friendly and efficient customer service support via chat, calls, emails, and other channels
-Familiarity with Minna’s Merchant Registry and classifications for merchants, services, and categories
-Proficiency in understanding subscription terms and pulling relevant information from internal systems to support Account Management, Sales, and other queries
-Conduct outbound calls to customers for subscription management and issue resolution
-Handle incoming queries from customers and merchants, ensuring timely resolution and escalation when necessary
-Collaborate with cross-functional teams to improve processes and enhance the customer experience
-Maintain accurate records and documentation of customer interactions and issue resolutions
-Based
-This role is based in Mumbai and will require daily commute.
-Requirements:
-Fluent in English with a minimum of 2-3 years of work experience in an International Call Center (US Voice Process or UK Voice Process)
-Comfortable working full-time in English and willing to work in US or UK shifts, must be flexible with work timings.
-Demonstrated ability to deliver excellent customer service and resolve issues with good judgment
-Strong analytical abilities for troubleshooting and problem-solving
-Appreciation for routine tasks and ability to follow clear instructions
-Comfortable multitasking to manage calls, emails, and chats simultaneously in an outbound calling process
-Strong communication skills, both verbal and written, with a friendly and professional tone
-Ability to adapt to a fast-paced and technologically advanced environment
-Detail-oriented with strong organizational skills and the ability to prioritize tasks effectively
-Our global benefits
-25 days holiday plus public holidays
-Private health insurance
-Subscription allowance
-Find more information about our benefits here
-Minna is an equal opportunities employer and does not discriminate on the basis of race, nationality, ethnicity, skin colour, religion, disability or sexual orientation. We celebrate and embrace a diverse workforce and are committed to building a team that represents a variety of backgrounds, perspectives and skills.</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>https://www.shl.com/solutions/products/product-catalog/view/professional-7-1-solution/</t>
-        </is>
-      </c>
-      <c r="C26" t="n">
-        <v>0.59</v>
-      </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>Matched due to overlap in key terms: manage, us, other, flexible, be, work, skills, deliver, as, not, will, professional, in, team, responsibilities, working, i, that, building, with, benefits, at, management, about, on, issues, providing, we, provide, communication, product, years, more, based, employer, sales, a, technology, or, when, this, is, ability, role, the, for, relevant, services, businesses, an, expert, leading, s, and, organizational, support, internal, opportunities, are, ensuring, teams, 2, by, strong, of, to, equal, experience</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>I want to hire Customer support executives who are expert in English communication.  
-We are looking for talented Customer Support specialists to join our Product operations team in India (Mumbai)
-Minna connects global banks and fintech with subscription businesses to give consumers self-serve subscription management in-app. Minna is a technology partner to top-tier financial institutions, fintech and subscription businesses, providing subscription management functionality for 50+ million banking and fintech customers across the United States, United Kingdom and Europe.
-Minna builds the infrastructure that links Subscription Merchants (such as Netflix, Spotify, Amazon) to leading Financial Institutions (Lloyds Bank, ING Belgium, Swedbank to name a few). This connection enables consumers to effortlessly manage their subscriptions by performing actions like canceling, pausing, or changing their plans.
-Responsibilities:
-Efficiently manage cancellations and monitor cancellation status for merchants
-Initiate and execute workflows for cancellations at various stages of the cancellation journey with merchants
-Provide friendly and efficient customer service support via chat, calls, emails, and other channels
-Familiarity with Minna’s Merchant Registry and classifications for merchants, services, and categories
-Proficiency in understanding subscription terms and pulling relevant information from internal systems to support Account Management, Sales, and other queries
-Conduct outbound calls to customers for subscription management and issue resolution
-Handle incoming queries from customers and merchants, ensuring timely resolution and escalation when necessary
-Collaborate with cross-functional teams to improve processes and enhance the customer experience
-Maintain accurate records and documentation of customer interactions and issue resolutions
-Based
-This role is based in Mumbai and will require daily commute.
-Requirements:
-Fluent in English with a minimum of 2-3 years of work experience in an International Call Center (US Voice Process or UK Voice Process)
-Comfortable working full-time in English and willing to work in US or UK shifts, must be flexible with work timings.
-Demonstrated ability to deliver excellent customer service and resolve issues with good judgment
-Strong analytical abilities for troubleshooting and problem-solving
-Appreciation for routine tasks and ability to follow clear instructions
-Comfortable multitasking to manage calls, emails, and chats simultaneously in an outbound calling process
-Strong communication skills, both verbal and written, with a friendly and professional tone
-Ability to adapt to a fast-paced and technologically advanced environment
-Detail-oriented with strong organizational skills and the ability to prioritize tasks effectively
-Our global benefits
-25 days holiday plus public holidays
-Private health insurance
-Subscription allowance
-Find more information about our benefits here
-Minna is an equal opportunities employer and does not discriminate on the basis of race, nationality, ethnicity, skin colour, religion, disability or sexual orientation. We celebrate and embrace a diverse workforce and are committed to building a team that represents a variety of backgrounds, perspectives and skills.</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>https://www.shl.com/solutions/products/product-catalog/view/shl-verify-interactive-numerical-calculation/</t>
-        </is>
-      </c>
-      <c r="C27" t="n">
-        <v>0.59</v>
-      </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>Matched due to overlap in key terms: manage, us, other, flexible, be, work, skills, deliver, as, not, will, professional, in, team, responsibilities, working, i, that, building, with, benefits, at, management, about, on, issues, providing, we, provide, communication, product, years, more, based, employer, sales, a, technology, or, when, this, is, ability, role, the, for, relevant, services, businesses, an, expert, leading, s, and, organizational, support, internal, opportunities, are, ensuring, teams, 2, by, strong, of, to, equal, experience</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>I want to hire Customer support executives who are expert in English communication.  
-We are looking for talented Customer Support specialists to join our Product operations team in India (Mumbai)
-Minna connects global banks and fintech with subscription businesses to give consumers self-serve subscription management in-app. Minna is a technology partner to top-tier financial institutions, fintech and subscription businesses, providing subscription management functionality for 50+ million banking and fintech customers across the United States, United Kingdom and Europe.
-Minna builds the infrastructure that links Subscription Merchants (such as Netflix, Spotify, Amazon) to leading Financial Institutions (Lloyds Bank, ING Belgium, Swedbank to name a few). This connection enables consumers to effortlessly manage their subscriptions by performing actions like canceling, pausing, or changing their plans.
-Responsibilities:
-Efficiently manage cancellations and monitor cancellation status for merchants
-Initiate and execute workflows for cancellations at various stages of the cancellation journey with merchants
-Provide friendly and efficient customer service support via chat, calls, emails, and other channels
-Familiarity with Minna’s Merchant Registry and classifications for merchants, services, and categories
-Proficiency in understanding subscription terms and pulling relevant information from internal systems to support Account Management, Sales, and other queries
-Conduct outbound calls to customers for subscription management and issue resolution
-Handle incoming queries from customers and merchants, ensuring timely resolution and escalation when necessary
-Collaborate with cross-functional teams to improve processes and enhance the customer experience
-Maintain accurate records and documentation of customer interactions and issue resolutions
-Based
-This role is based in Mumbai and will require daily commute.
-Requirements:
-Fluent in English with a minimum of 2-3 years of work experience in an International Call Center (US Voice Process or UK Voice Process)
-Comfortable working full-time in English and willing to work in US or UK shifts, must be flexible with work timings.
-Demonstrated ability to deliver excellent customer service and resolve issues with good judgment
-Strong analytical abilities for troubleshooting and problem-solving
-Appreciation for routine tasks and ability to follow clear instructions
-Comfortable multitasking to manage calls, emails, and chats simultaneously in an outbound calling process
-Strong communication skills, both verbal and written, with a friendly and professional tone
-Ability to adapt to a fast-paced and technologically advanced environment
-Detail-oriented with strong organizational skills and the ability to prioritize tasks effectively
-Our global benefits
-25 days holiday plus public holidays
-Private health insurance
-Subscription allowance
-Find more information about our benefits here
-Minna is an equal opportunities employer and does not discriminate on the basis of race, nationality, ethnicity, skin colour, religion, disability or sexual orientation. We celebrate and embrace a diverse workforce and are committed to building a team that represents a variety of backgrounds, perspectives and skills.</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>https://www.shl.com/solutions/products/product-catalog/view/administrative-professional-short-form/</t>
-        </is>
-      </c>
-      <c r="C28" t="n">
-        <v>0.59</v>
-      </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>Matched due to overlap in key terms: manage, us, other, flexible, be, work, skills, deliver, as, not, will, professional, in, team, responsibilities, working, i, that, building, with, benefits, at, management, about, on, issues, providing, we, provide, communication, product, years, more, based, employer, sales, a, technology, or, when, this, is, ability, role, the, for, relevant, services, businesses, an, expert, leading, s, and, organizational, support, internal, opportunities, are, ensuring, teams, 2, by, strong, of, to, equal, experience</t>
-        </is>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Sql Server New</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>https://www.shl.com/solutions/products/product-catalog/view/sql-server-new/</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>0.663</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Recommended because the job description shares key focus areas such as 40, range, investment, adjustments, application, outcomes, transformation, culture, shlhiringtalent, and, in, help, workplace, lead, can, with, breaking, for, product, doing, management, years, providing, scale, employee, sure, processes, your, assessment, all, path, greatest, goals, possible, friendly, benefits, candidates, achieve, package, the, people, threads, more, part, strong, excellent, currently, job, market, business, touch, power, ability, is, description, me, are, time, world, growth, an, when, accessibility, coaching, better, develop, flexibility, huge, how, below, acquisition, than, ongoing, guidance, this, our, on, started, dei, support, become, success, at, shl, flexible, ll, transform, experience, looking, find, out, ago, of, work, ground, inclusivity, possibilities, unlock, we, continue, choose, key, what, there, lifeatshl, you, off, fabric, get, one, recruitment, businesses, join, offered, career, from, diversity, intrinsic, careersatshl, talent, something, technology, insights, do, by, industry, or, inspire, transformational, experiences, no, diverse, inspired, insight, s, family, team, 1, that, collaboration, products, quality, knowledge, through, powerhouse, inclusive, about, services, development, make, where, knowledgeable, inclusion, others, so, opportunity, making, us, care, launches, a, will, encourage, employer, manager, takes, lives, as, offer, new, equity, best, applications, science, process, around, answers, equal, be, workplaces, fun, to</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Metric</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Value</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Total Queries</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Avg Similarity</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0.524</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Top Match Confidence</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0.75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>